<commit_message>
Fix font. Extend size of the SN columns
</commit_message>
<xml_diff>
--- a/Plantilla_Guia_ENV-OBIS_vSM2021.1.xlsx
+++ b/Plantilla_Guia_ENV-OBIS_vSM2021.1.xlsx
@@ -751,7 +751,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="39">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -840,13 +840,6 @@
       <i val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFCCCCCC"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -1319,20 +1312,24 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1343,15 +1340,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1359,7 +1352,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1367,11 +1360,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1379,19 +1372,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1399,36 +1392,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1436,18 +1433,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1455,27 +1448,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1483,15 +1476,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1499,7 +1488,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1511,7 +1504,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1519,7 +1512,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1527,7 +1520,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1543,7 +1536,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1555,95 +1548,95 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1651,15 +1644,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1746,9 +1739,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>651600</xdr:colOff>
+      <xdr:colOff>651240</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1761,8 +1754,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1947960" y="2133360"/>
-          <a:ext cx="4848840" cy="3388680"/>
+          <a:off x="1949040" y="2133360"/>
+          <a:ext cx="4855320" cy="3388320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1783,9 +1776,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>48960</xdr:colOff>
+      <xdr:colOff>48600</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1798,8 +1791,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1528920" y="352080"/>
-          <a:ext cx="2616840" cy="950400"/>
+          <a:off x="1530000" y="352080"/>
+          <a:ext cx="2620440" cy="950040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1820,9 +1813,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
+      <xdr:colOff>258120</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1835,8 +1828,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5130360" y="352080"/>
-          <a:ext cx="3322080" cy="950400"/>
+          <a:off x="5136840" y="352080"/>
+          <a:ext cx="3325320" cy="950040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2153,10 +2146,10 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="40.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="33.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="20.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="19.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="41.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="58.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="23.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="24.63"/>
@@ -5263,16 +5256,16 @@
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true" selectLockedCells="true"/>
   <dataValidations count="3">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1001" type="list">
+      <formula1>'Event (Evento)'!$A$2:$A$10000</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C1001" type="list">
       <formula1>"PreservedSpecimen,FossilSpecimen,LivingSpecimen,HumanObservation,MachineObservation"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D1001" type="list">
       <formula1>"Present,Absent"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1001" type="list">
-      <formula1>'Event (Evento)'!$A$2:$A$10000</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -8394,7 +8387,7 @@
       <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>
@@ -13052,7 +13045,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="59"/>
@@ -13257,7 +13250,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>
@@ -15076,7 +15069,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.69"/>

</xml_diff>